<commit_message>
Edited Sample .xlsx file
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahimnpatel/Documents/Dev/votingsystem/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9348E2E6-A785-8747-9F9F-9853168FC062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE03884-159F-F441-B72C-4DA5DA1B5D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="500" windowWidth="37460" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="320">
   <si>
     <t>First Name</t>
   </si>
@@ -980,27 +980,6 @@
   </si>
   <si>
     <t>btame1d@apple.com</t>
-  </si>
-  <si>
-    <t>Mahimn</t>
-  </si>
-  <si>
-    <t>Patel</t>
-  </si>
-  <si>
-    <t>Borrelli</t>
-  </si>
-  <si>
-    <t>Brampton</t>
-  </si>
-  <si>
-    <t>L6Y5X1</t>
-  </si>
-  <si>
-    <t>437-438-7554</t>
-  </si>
-  <si>
-    <t>kingmahimn@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1363,7 +1342,7 @@
   <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2930,41 +2909,9 @@
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A52" t="s">
-        <v>320</v>
-      </c>
-      <c r="B52" t="s">
-        <v>321</v>
-      </c>
-      <c r="C52">
-        <v>76</v>
-      </c>
-      <c r="D52" t="s">
-        <v>322</v>
-      </c>
-      <c r="E52" t="s">
-        <v>323</v>
-      </c>
-      <c r="F52" t="s">
-        <v>324</v>
-      </c>
-      <c r="G52" t="s">
-        <v>325</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="I52" t="b">
-        <v>0</v>
-      </c>
-      <c r="J52" t="s">
-        <v>17</v>
-      </c>
+      <c r="H52" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H52" r:id="rId1" xr:uid="{41CB9353-4803-BC4C-AB08-CE551D97E578}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>